<commit_message>
Writed Result Test Case & Threads
</commit_message>
<xml_diff>
--- a/App_TestWithdrawFund/result_threads.xlsx
+++ b/App_TestWithdrawFund/result_threads.xlsx
@@ -1,11 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
-  <sheets/>
+  <sheets>
+    <sheet name="sheet1" r:id="rId3" sheetId="1"/>
+  </sheets>
 </workbook>
 </file>
 
@@ -49,4 +51,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="true"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>